<commit_message>
add combine result, update usermanual
</commit_message>
<xml_diff>
--- a/Program/condition.xlsx
+++ b/Program/condition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_filtering\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548CC5C0-6C4E-4E0B-B23C-64F7DC124837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF1142-920F-4A32-865A-725871AF4FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add combine result, change condition
</commit_message>
<xml_diff>
--- a/Program/condition.xlsx
+++ b/Program/condition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_filtering\Program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\student\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01792AA2-A1AF-4CE6-B7F3-8DCEF2624DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0E997-C3A5-4D0D-8159-C2C66206CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fix exclude for segment
</commit_message>
<xml_diff>
--- a/Program/condition.xlsx
+++ b/Program/condition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\student\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0E997-C3A5-4D0D-8159-C2C66206CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C394B714-848D-4816-BC47-DEE2952C96D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Revert "fix exclude for segment"
This reverts commit 1e1ffee4d0453719af0cae0c315d84a224e7ded5.
</commit_message>
<xml_diff>
--- a/Program/condition.xlsx
+++ b/Program/condition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\student\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C394B714-848D-4816-BC47-DEE2952C96D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0E997-C3A5-4D0D-8159-C2C66206CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>